<commit_message>
add: results after run notebook last time
</commit_message>
<xml_diff>
--- a/errors_table/errorsTable_15min_LSTM_maeLoss.xlsx
+++ b/errors_table/errorsTable_15min_LSTM_maeLoss.xlsx
@@ -775,100 +775,100 @@
         <v>8</v>
       </c>
       <c r="E5" t="n">
-        <v>0.013017267</v>
+        <v>0.0150041999</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0003350181</v>
+        <v>0.0004644361</v>
       </c>
       <c r="G5" t="n">
-        <v>0.09032869340000001</v>
+        <v>0.1127824783</v>
       </c>
       <c r="H5" t="n">
-        <v>4.0984663963</v>
+        <v>5.2422862053</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0143599976</v>
+        <v>0.0193367973</v>
       </c>
       <c r="J5" t="n">
-        <v>0.0005227312</v>
+        <v>0.0009260924</v>
       </c>
       <c r="K5" t="n">
-        <v>0.1337336302</v>
+        <v>0.1941526532</v>
       </c>
       <c r="L5" t="n">
-        <v>9.1457614899</v>
+        <v>14.5507297516</v>
       </c>
       <c r="M5" t="n">
-        <v>0.07340810146463411</v>
+        <v>0.08713245520243898</v>
       </c>
       <c r="N5" t="n">
-        <v>0.01084120323679338</v>
+        <v>0.01322879565028934</v>
       </c>
       <c r="O5" t="n">
-        <v>0.3738010825</v>
+        <v>0.3662151112999998</v>
       </c>
       <c r="P5" t="n">
-        <v>0.01577159120654701</v>
+        <v>0.01917805240263791</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.1471455302463415</v>
+        <v>0.2049857087914634</v>
       </c>
       <c r="R5" t="n">
-        <v>0.03074692410535063</v>
+        <v>0.04998100075705328</v>
       </c>
       <c r="S5" t="n">
-        <v>0.4559996869000003</v>
+        <v>0.4581298399999998</v>
       </c>
       <c r="T5" t="n">
-        <v>0.03070735453534065</v>
+        <v>0.04484785861462664</v>
       </c>
       <c r="U5" t="n">
-        <v>0.08472918057560991</v>
+        <v>0.09358293865731712</v>
       </c>
       <c r="V5" t="n">
-        <v>0.01248035575685384</v>
+        <v>0.01512463012686926</v>
       </c>
       <c r="W5" t="n">
-        <v>0.3563977511999994</v>
+        <v>0.3930178176000005</v>
       </c>
       <c r="X5" t="n">
-        <v>0.01171603986015334</v>
+        <v>0.01288598188120367</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.1036227231000001</v>
+        <v>0.1571766717621952</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.01744047403294654</v>
+        <v>0.03214146853309562</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.3728504221000009</v>
+        <v>0.4359028488999996</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.01486128729903133</v>
+        <v>0.02223979184531321</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.07652790779103481</v>
+        <v>0.08520624953354147</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.009197122629718103</v>
+        <v>0.01082621235206209</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.3924444153</v>
+        <v>0.4116257720999998</v>
       </c>
       <c r="AF5" t="n">
-        <v>0.01553163943379163</v>
+        <v>0.01730429481936817</v>
       </c>
       <c r="AG5" t="n">
-        <v>0.177313968938537</v>
+        <v>0.215171872347636</v>
       </c>
       <c r="AH5" t="n">
-        <v>0.03573904102137088</v>
+        <v>0.05024528974572511</v>
       </c>
       <c r="AI5" t="n">
-        <v>0.4861516021000005</v>
+        <v>0.5421935017999999</v>
       </c>
       <c r="AJ5" t="n">
-        <v>0.03606477543037612</v>
+        <v>0.04373778559697056</v>
       </c>
     </row>
     <row r="6">
@@ -887,100 +887,100 @@
         <v>16</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0174059886</v>
+        <v>0.0134369098</v>
       </c>
       <c r="F6" t="n">
-        <v>0.00071481</v>
+        <v>0.0003546652</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1470702589</v>
+        <v>0.078820318</v>
       </c>
       <c r="H6" t="n">
-        <v>5.6080064774</v>
+        <v>4.3206686974</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0186796319</v>
+        <v>0.0184779037</v>
       </c>
       <c r="J6" t="n">
-        <v>0.0010996538</v>
+        <v>0.0007264043</v>
       </c>
       <c r="K6" t="n">
-        <v>0.2132236362</v>
+        <v>0.1395274401</v>
       </c>
       <c r="L6" t="n">
-        <v>12.5378646851</v>
+        <v>15.690653801</v>
       </c>
       <c r="M6" t="n">
-        <v>0.0738992676268293</v>
+        <v>0.09365449193048778</v>
       </c>
       <c r="N6" t="n">
-        <v>0.01280126558683236</v>
+        <v>0.01364614231864257</v>
       </c>
       <c r="O6" t="n">
-        <v>0.360858146</v>
+        <v>0.3431521409</v>
       </c>
       <c r="P6" t="n">
-        <v>0.01604968130965899</v>
+        <v>0.02095367475148259</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.1137705539256098</v>
+        <v>0.2871720668256098</v>
       </c>
       <c r="R6" t="n">
-        <v>0.02850441061122369</v>
+        <v>0.09924895117487342</v>
       </c>
       <c r="S6" t="n">
-        <v>0.6331380751999998</v>
+        <v>0.5757091534000001</v>
       </c>
       <c r="T6" t="n">
-        <v>0.02459179362704021</v>
+        <v>0.06378066916460212</v>
       </c>
       <c r="U6" t="n">
-        <v>0.09685707538780487</v>
+        <v>0.08409094357682924</v>
       </c>
       <c r="V6" t="n">
-        <v>0.0182517024771235</v>
+        <v>0.01235060334705156</v>
       </c>
       <c r="W6" t="n">
-        <v>0.3882775596999997</v>
+        <v>0.3420374807000002</v>
       </c>
       <c r="X6" t="n">
-        <v>0.01304948457820916</v>
+        <v>0.01180574616415395</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.2124381140573171</v>
+        <v>0.1384540965536586</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.1220791462719739</v>
+        <v>0.03034102997371167</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.9345520131000002</v>
+        <v>0.4383362913000006</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.0279600992077929</v>
+        <v>0.02168252878731586</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.05411510949214986</v>
+        <v>0.08318048070847457</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.005240792030545934</v>
+        <v>0.01047380758161532</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.3882775596999997</v>
+        <v>0.4135514535000002</v>
       </c>
       <c r="AF6" t="n">
-        <v>0.01086070266435501</v>
+        <v>0.01693586533446379</v>
       </c>
       <c r="AG6" t="n">
-        <v>0.07009413974272971</v>
+        <v>0.4277105660935772</v>
       </c>
       <c r="AH6" t="n">
-        <v>0.01157983306558142</v>
+        <v>0.1906173135636298</v>
       </c>
       <c r="AI6" t="n">
-        <v>0.93430049</v>
+        <v>0.7572189151000002</v>
       </c>
       <c r="AJ6" t="n">
-        <v>0.01388045887696081</v>
+        <v>0.08721984374706636</v>
       </c>
     </row>
     <row r="7">

</xml_diff>